<commit_message>
changed to absolute path
</commit_message>
<xml_diff>
--- a/2.詳細設計/システム構築マニュアル.xlsx
+++ b/2.詳細設計/システム構築マニュアル.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\kanjitest\2.詳細設計\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3F0BE2-E593-4819-985F-FD86C7EF85E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7FEF79-D93B-4DC8-806F-E008A0935960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,10 +64,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>cd /kanjitest/backend</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>cd ../client</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -243,6 +239,10 @@
   </si>
   <si>
     <t>sudo node index.js</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cd kanjitest/backend</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -610,7 +610,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -620,12 +622,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -640,7 +642,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -650,7 +652,7 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -660,7 +662,7 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -670,17 +672,17 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="4" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -690,17 +692,17 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -713,52 +715,52 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:1">
@@ -768,17 +770,17 @@
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>